<commit_message>
ED slideshows all up
</commit_message>
<xml_diff>
--- a/resources/docs/slide-show calculations.xlsx
+++ b/resources/docs/slide-show calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\programs\christopher-cattron-professional-portfolio\resources\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA0C092C-6841-4D1F-8D30-A3E147CB09EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D57466D-65F3-40D8-8B0D-CD05C45198DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{497367ED-7BF3-403F-8B15-C8DE285259D2}"/>
+    <workbookView xWindow="-11616" yWindow="5028" windowWidth="17280" windowHeight="8964" xr2:uid="{497367ED-7BF3-403F-8B15-C8DE285259D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>                        0%,</t>
   </si>
@@ -436,6 +436,12 @@
   </si>
   <si>
     <t>img</t>
+  </si>
+  <si>
+    <t>int 7</t>
+  </si>
+  <si>
+    <t>step 12.5</t>
   </si>
 </sst>
 </file>
@@ -820,15 +826,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE556419-7304-4ACC-A917-2C4DC5C4E046}">
-  <dimension ref="D6:X39"/>
+  <dimension ref="D6:AE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AC10" sqref="AC10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="6" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:31" x14ac:dyDescent="0.3">
       <c r="M6" t="s">
         <v>24</v>
       </c>
@@ -841,8 +847,32 @@
       <c r="P6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="4:24" x14ac:dyDescent="0.3">
+      <c r="V6" t="s">
+        <v>24</v>
+      </c>
+      <c r="W6" t="s">
+        <v>23</v>
+      </c>
+      <c r="X6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D7" s="1" t="s">
         <v>0</v>
       </c>
@@ -869,16 +899,31 @@
         <v>7</v>
       </c>
       <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
         <v>11.2</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>0</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="4:24" x14ac:dyDescent="0.3">
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>18.666666666666664</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D8" s="1" t="s">
         <v>1</v>
       </c>
@@ -905,17 +950,33 @@
         <v>12.5</v>
       </c>
       <c r="V8">
-        <f>V7+20</f>
+        <v>20</v>
+      </c>
+      <c r="W8">
+        <f>W7+20</f>
         <v>31.2</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>-20</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="4:24" x14ac:dyDescent="0.3">
+      <c r="AB8">
+        <v>33.333300000000001</v>
+      </c>
+      <c r="AC8">
+        <f>AC7+AB8</f>
+        <v>51.999966666666666</v>
+      </c>
+      <c r="AD8">
+        <v>-33.332999999999998</v>
+      </c>
+      <c r="AE8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D9" s="1" t="s">
         <v>2</v>
       </c>
@@ -942,17 +1003,33 @@
         <v>12.5</v>
       </c>
       <c r="V9">
-        <f t="shared" ref="V9:V11" si="1">V8+20</f>
+        <v>40</v>
+      </c>
+      <c r="W9">
+        <f t="shared" ref="W9:W11" si="1">W8+20</f>
         <v>51.2</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>-40</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="4:24" x14ac:dyDescent="0.3">
+      <c r="AB9">
+        <v>66.666700000000006</v>
+      </c>
+      <c r="AC9">
+        <f>AC7+AB9</f>
+        <v>85.333366666666677</v>
+      </c>
+      <c r="AD9">
+        <v>-66.667000000000002</v>
+      </c>
+      <c r="AE9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
@@ -979,17 +1056,20 @@
         <v>12.5</v>
       </c>
       <c r="V10">
+        <v>60</v>
+      </c>
+      <c r="W10">
         <f t="shared" si="1"/>
         <v>71.2</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>-60</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1016,17 +1096,20 @@
         <v>12.5</v>
       </c>
       <c r="V11">
+        <v>80</v>
+      </c>
+      <c r="W11">
         <f t="shared" si="1"/>
         <v>91.2</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>-80</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1050,7 +1133,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="13" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D13" s="1" t="s">
         <v>6</v>
       </c>
@@ -1074,7 +1157,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="14" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1098,40 +1181,50 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="15" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D15" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="4:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="U18">
+      <c r="N18" t="s">
+        <v>26</v>
+      </c>
+      <c r="V18">
         <f>7/12.5</f>
         <v>0.56000000000000005</v>
       </c>
-      <c r="V18">
-        <f>20*U18</f>
+      <c r="W18">
+        <f>20*V18</f>
         <v>11.200000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="Z18">
+        <f>11.2/20</f>
+        <v>0.55999999999999994</v>
+      </c>
+    </row>
+    <row r="19" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D19" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="N19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D20" s="1" t="s">
         <v>11</v>
       </c>
@@ -1139,63 +1232,71 @@
         <f>100/8</f>
         <v>12.5</v>
       </c>
-    </row>
-    <row r="21" spans="4:22" x14ac:dyDescent="0.3">
+      <c r="AC20">
+        <f>100/3</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="AD20">
+        <f>AC20*Z18</f>
+        <v>18.666666666666664</v>
+      </c>
+    </row>
+    <row r="21" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D21" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D22" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D23" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D24" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D25" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D26" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D27" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D28" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D29" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D30" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D31" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:30" x14ac:dyDescent="0.3">
       <c r="D32" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Add projects to the FUN ZONE; changed h3 headings to h2
</commit_message>
<xml_diff>
--- a/resources/docs/slide-show calculations.xlsx
+++ b/resources/docs/slide-show calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\programs\christopher-cattron-professional-portfolio\resources\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D57466D-65F3-40D8-8B0D-CD05C45198DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4B5CF4-F37E-4974-8AEC-57CDB65D2EED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11616" yWindow="5028" windowWidth="17280" windowHeight="8964" xr2:uid="{497367ED-7BF3-403F-8B15-C8DE285259D2}"/>
+    <workbookView xWindow="-552" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{497367ED-7BF3-403F-8B15-C8DE285259D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -828,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE556419-7304-4ACC-A917-2C4DC5C4E046}">
   <dimension ref="D6:AE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AC10" sqref="AC10"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AE13" sqref="AE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -963,11 +963,11 @@
         <v>2</v>
       </c>
       <c r="AB8">
-        <v>33.333300000000001</v>
+        <v>33.333333330000002</v>
       </c>
       <c r="AC8">
         <f>AC7+AB8</f>
-        <v>51.999966666666666</v>
+        <v>51.999999996666666</v>
       </c>
       <c r="AD8">
         <v>-33.332999999999998</v>
@@ -1016,11 +1016,11 @@
         <v>3</v>
       </c>
       <c r="AB9">
-        <v>66.666700000000006</v>
+        <v>66.6666666666666</v>
       </c>
       <c r="AC9">
         <f>AC7+AB9</f>
-        <v>85.333366666666677</v>
+        <v>85.333333333333258</v>
       </c>
       <c r="AD9">
         <v>-66.667000000000002</v>

</xml_diff>